<commit_message>
'Add Test for Keyword Setup'
</commit_message>
<xml_diff>
--- a/Code/Book1.xlsx
+++ b/Code/Book1.xlsx
@@ -48,7 +48,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -59,6 +59,12 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -90,33 +96,45 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -430,55 +448,55 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="7" width="10.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="9" width="17.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="11" width="10.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="11" width="17.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="7">
         <v>1000</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="8">
         <v>0.7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="1"/>
-      <c r="B3" s="5" t="s">
+      <c r="A3" s="9"/>
+      <c r="B3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="4"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add new input excel
</commit_message>
<xml_diff>
--- a/Code/Book1.xlsx
+++ b/Code/Book1.xlsx
@@ -14,33 +14,84 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>CamName</t>
-  </si>
-  <si>
-    <t>Asin</t>
-  </si>
-  <si>
-    <t>DailyBudget</t>
-  </si>
-  <si>
-    <t>ProductName</t>
-  </si>
-  <si>
-    <t>Bid</t>
-  </si>
-  <si>
-    <t>ABC1</t>
-  </si>
-  <si>
-    <t>SA001</t>
-  </si>
-  <si>
-    <t>Example</t>
-  </si>
-  <si>
-    <t>SA002</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
+  <si>
+    <t>CampName</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Entity</t>
+  </si>
+  <si>
+    <t>ASIN/SKU</t>
+  </si>
+  <si>
+    <t>Targeting</t>
+  </si>
+  <si>
+    <t>budget</t>
+  </si>
+  <si>
+    <t>bid</t>
+  </si>
+  <si>
+    <t>matchtype</t>
+  </si>
+  <si>
+    <t>Cost type</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>SP</t>
+  </si>
+  <si>
+    <t>Keyword</t>
+  </si>
+  <si>
+    <t>B0ABCXYZHG</t>
+  </si>
+  <si>
+    <t>wall basket decor</t>
+  </si>
+  <si>
+    <t>Exact</t>
+  </si>
+  <si>
+    <t>product targeting</t>
+  </si>
+  <si>
+    <t>B09BCXYZHG</t>
+  </si>
+  <si>
+    <t>ABRAND</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>Audience targeting</t>
+  </si>
+  <si>
+    <t>audience="360733347960105375"</t>
+  </si>
+  <si>
+    <t>T00030</t>
+  </si>
+  <si>
+    <t>CPC</t>
+  </si>
+  <si>
+    <t>Contextual targeting</t>
+  </si>
+  <si>
+    <t>T00020</t>
+  </si>
+  <si>
+    <t>vCPM</t>
   </si>
 </sst>
 </file>
@@ -48,19 +99,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -96,7 +141,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -113,32 +158,44 @@
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -442,20 +499,24 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="11" width="10.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="11" width="17.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="15" width="27.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="15" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="16" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="17" width="18.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="17" width="21.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="17" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="17" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="17" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="18" width="20.290714285714284" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -468,35 +529,129 @@
       <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="8">
+        <v>15</v>
+      </c>
+      <c r="G2" s="8">
+        <v>1</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18">
+      <c r="A3" s="10"/>
+      <c r="B3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="8">
+        <v>10</v>
+      </c>
+      <c r="G3" s="12">
+        <v>0.7</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="13"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18">
+      <c r="A4" s="10"/>
+      <c r="B4" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="8">
+        <v>15</v>
+      </c>
+      <c r="G4" s="8">
+        <v>1</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+      <c r="A5" s="7"/>
+      <c r="B5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="8">
+        <v>15</v>
+      </c>
+      <c r="G5" s="8">
         <v>5</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="7">
-        <v>1000</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="8">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="9"/>
-      <c r="B3" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="10"/>
+      <c r="H5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" s="14" t="s">
+        <v>25</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>